<commit_message>
Updated User Story BL054. All tests complete, waiting for acceptance criteria. Started task BLL42. Completed definition and initialisation of Measure class ready for TM to use in Sprint 3.
git-svn-id: https://sfs.atcorau.local/svn/SoftwareRepository/trunk@184 a8a9b14d-6b92-5b4b-9153-4cd90bb22c97
</commit_message>
<xml_diff>
--- a/PN022BLL/biz/Debug/Data1.xlsx
+++ b/PN022BLL/biz/Debug/Data1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="24795" windowHeight="12165"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="15600" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>PWV_09</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>CalculatedDistance</t>
+  </si>
+  <si>
+    <t>Re-Work</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Deltas</t>
+  </si>
+  <si>
+    <t>Valid Deltas</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>MeanDeltaTime (points)</t>
   </si>
 </sst>
 </file>
@@ -386,27 +404,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -435,7 +455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -467,7 +487,7 @@
         <v>5118</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -499,7 +519,7 @@
         <v>5118</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -531,12 +551,12 @@
         <v>5118</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -568,7 +588,7 @@
         <v>5118</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -600,7 +620,7 @@
         <v>5118</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -630,6 +650,426 @@
       </c>
       <c r="J9">
         <v>5118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>82</v>
+      </c>
+      <c r="C13">
+        <v>42</v>
+      </c>
+      <c r="D13">
+        <v>600</v>
+      </c>
+      <c r="E13">
+        <v>400</v>
+      </c>
+      <c r="F13">
+        <v>9.6</v>
+      </c>
+      <c r="G13">
+        <v>0.4</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>56</v>
+      </c>
+      <c r="J13">
+        <v>2730</v>
+      </c>
+      <c r="K13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>68</v>
+      </c>
+      <c r="C14">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>530</v>
+      </c>
+      <c r="E14">
+        <v>330</v>
+      </c>
+      <c r="F14">
+        <v>11.7</v>
+      </c>
+      <c r="G14">
+        <v>0.5</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>65</v>
+      </c>
+      <c r="J14">
+        <v>2350</v>
+      </c>
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>126</v>
+      </c>
+      <c r="C15">
+        <v>87</v>
+      </c>
+      <c r="D15">
+        <v>740</v>
+      </c>
+      <c r="E15">
+        <v>540</v>
+      </c>
+      <c r="F15">
+        <v>6.3</v>
+      </c>
+      <c r="G15">
+        <v>0.7</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>58</v>
+      </c>
+      <c r="J15">
+        <v>2640</v>
+      </c>
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>68.359375</v>
+      </c>
+      <c r="C18">
+        <v>28.359375</v>
+      </c>
+      <c r="D18">
+        <v>600</v>
+      </c>
+      <c r="E18">
+        <v>400</v>
+      </c>
+      <c r="F18">
+        <v>14.969249</v>
+      </c>
+      <c r="G18">
+        <v>3.7568695999999999</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>56.298214000000002</v>
+      </c>
+      <c r="J18">
+        <v>2730</v>
+      </c>
+      <c r="K18">
+        <v>8</v>
+      </c>
+      <c r="L18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>61.197918000000001</v>
+      </c>
+      <c r="C19">
+        <v>21.197915999999999</v>
+      </c>
+      <c r="D19">
+        <v>530</v>
+      </c>
+      <c r="E19">
+        <v>330</v>
+      </c>
+      <c r="F19">
+        <v>15.693745</v>
+      </c>
+      <c r="G19">
+        <v>1.4525071000000001</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>65.362487999999999</v>
+      </c>
+      <c r="J19">
+        <v>2350</v>
+      </c>
+      <c r="K19">
+        <v>8</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>106.93359</v>
+      </c>
+      <c r="C20">
+        <v>66.933593999999999</v>
+      </c>
+      <c r="D20">
+        <v>740</v>
+      </c>
+      <c r="E20">
+        <v>540</v>
+      </c>
+      <c r="F20">
+        <v>8.3078651000000008</v>
+      </c>
+      <c r="G20">
+        <v>1.5169550000000001</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>58.082222000000002</v>
+      </c>
+      <c r="J20">
+        <v>2640</v>
+      </c>
+      <c r="K20">
+        <v>8</v>
+      </c>
+      <c r="L20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="B23">
+        <v>62.5</v>
+      </c>
+      <c r="C23">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>22.5</v>
+      </c>
+      <c r="E23">
+        <v>14.666667</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="B24">
+        <v>62.5</v>
+      </c>
+      <c r="C24">
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>22.5</v>
+      </c>
+      <c r="E24">
+        <v>14.666667</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="B25">
+        <v>58.59375</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>18.59375</v>
+      </c>
+      <c r="E25">
+        <v>17.747900000000001</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="B26">
+        <v>50.78125</v>
+      </c>
+      <c r="C26">
+        <v>13</v>
+      </c>
+      <c r="D26">
+        <v>10.78125</v>
+      </c>
+      <c r="E26">
+        <v>30.608695999999998</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="B27">
+        <v>50.78125</v>
+      </c>
+      <c r="C27">
+        <v>13</v>
+      </c>
+      <c r="D27">
+        <v>10.78125</v>
+      </c>
+      <c r="E27">
+        <v>30.608695999999998</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="B28">
+        <v>42.96875</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>2.96875</v>
+      </c>
+      <c r="E28">
+        <v>111.1579</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="B29">
+        <v>39.0625</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>-0.9375</v>
+      </c>
+      <c r="E29">
+        <v>-1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="B30">
+        <v>35.15625</v>
+      </c>
+      <c r="C30">
+        <v>9</v>
+      </c>
+      <c r="D30">
+        <v>-4.84375</v>
+      </c>
+      <c r="E30">
+        <v>-1</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User Story BL054 complete and acceptance criteria met. Committed for peer review.
git-svn-id: https://sfs.atcorau.local/svn/SoftwareRepository/trunk@189 a8a9b14d-6b92-5b4b-9153-4cd90bb22c97
</commit_message>
<xml_diff>
--- a/PN022BLL/biz/Debug/Data1.xlsx
+++ b/PN022BLL/biz/Debug/Data1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="20">
   <si>
     <t>PWV_09</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>MeanDeltaTime (points)</t>
+  </si>
+  <si>
+    <t>Take 3!</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1070,6 +1073,270 @@
       </c>
       <c r="F30" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" t="s">
+        <v>8</v>
+      </c>
+      <c r="I33" t="s">
+        <v>2</v>
+      </c>
+      <c r="J33" t="s">
+        <v>5</v>
+      </c>
+      <c r="K33" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>82</v>
+      </c>
+      <c r="C34">
+        <v>42</v>
+      </c>
+      <c r="D34">
+        <v>600</v>
+      </c>
+      <c r="E34">
+        <v>400</v>
+      </c>
+      <c r="F34">
+        <v>9.6</v>
+      </c>
+      <c r="G34">
+        <v>0.4</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>56</v>
+      </c>
+      <c r="J34">
+        <v>2730</v>
+      </c>
+      <c r="K34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>68</v>
+      </c>
+      <c r="C35">
+        <v>28</v>
+      </c>
+      <c r="D35">
+        <v>530</v>
+      </c>
+      <c r="E35">
+        <v>330</v>
+      </c>
+      <c r="F35">
+        <v>11.7</v>
+      </c>
+      <c r="G35">
+        <v>0.5</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>65</v>
+      </c>
+      <c r="J35">
+        <v>2350</v>
+      </c>
+      <c r="K35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>126</v>
+      </c>
+      <c r="C36">
+        <v>87</v>
+      </c>
+      <c r="D36">
+        <v>740</v>
+      </c>
+      <c r="E36">
+        <v>540</v>
+      </c>
+      <c r="F36">
+        <v>6.3</v>
+      </c>
+      <c r="G36">
+        <v>0.7</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>58</v>
+      </c>
+      <c r="J36">
+        <v>2640</v>
+      </c>
+      <c r="K36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>80.861557000000005</v>
+      </c>
+      <c r="C39">
+        <v>40.861556999999998</v>
+      </c>
+      <c r="D39">
+        <v>600</v>
+      </c>
+      <c r="E39">
+        <v>400</v>
+      </c>
+      <c r="F39">
+        <v>9.8067969999999995</v>
+      </c>
+      <c r="G39">
+        <v>0.42628961999999998</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>56.263924000000003</v>
+      </c>
+      <c r="J39">
+        <v>2730</v>
+      </c>
+      <c r="K39">
+        <v>8</v>
+      </c>
+      <c r="L39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>67.484497000000005</v>
+      </c>
+      <c r="C40">
+        <v>27.484497000000001</v>
+      </c>
+      <c r="D40">
+        <v>530</v>
+      </c>
+      <c r="E40">
+        <v>330</v>
+      </c>
+      <c r="F40">
+        <v>12.061915000000001</v>
+      </c>
+      <c r="G40">
+        <v>0.80147111000000004</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>65.327667000000005</v>
+      </c>
+      <c r="J40">
+        <v>2350</v>
+      </c>
+      <c r="K40">
+        <v>8</v>
+      </c>
+      <c r="L40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>124.31859</v>
+      </c>
+      <c r="C41">
+        <v>84.318588000000005</v>
+      </c>
+      <c r="D41">
+        <v>740</v>
+      </c>
+      <c r="E41">
+        <v>540</v>
+      </c>
+      <c r="F41">
+        <v>6.4872775000000003</v>
+      </c>
+      <c r="G41">
+        <v>0.71557104999999999</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>58.082222000000002</v>
+      </c>
+      <c r="J41">
+        <v>2640</v>
+      </c>
+      <c r="K41">
+        <v>8</v>
+      </c>
+      <c r="L41">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>